<commit_message>
updated data; trying multi-file input
</commit_message>
<xml_diff>
--- a/Endpoint_rename/data/S5_N7_PCR-run1.xlsx
+++ b/Endpoint_rename/data/S5_N7_PCR-run1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="20000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SYBR" sheetId="1" r:id="rId1"/>
@@ -1135,8 +1135,8 @@
   <dimension ref="A1:K97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B63" state="frozen"/>
-      <selection activeCell="M89" sqref="M89"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B64" state="frozen"/>
+      <selection activeCell="M82" sqref="M82"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
@@ -1234,9 +1234,6 @@
       <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="8">
-        <v>10000</v>
-      </c>
       <c r="H3" s="9" t="s">
         <v>12</v>
       </c>
@@ -1263,9 +1260,6 @@
       <c r="E4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="8">
-        <v>10000</v>
-      </c>
       <c r="H4" s="9" t="s">
         <v>12</v>
       </c>
@@ -1293,9 +1287,6 @@
         <v>13</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="8">
-        <v>10000</v>
-      </c>
       <c r="H5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1323,9 +1314,6 @@
         <v>13</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="8">
-        <v>10000</v>
-      </c>
       <c r="H6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1353,9 +1341,6 @@
         <v>13</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="8">
-        <v>10000</v>
-      </c>
       <c r="H7" s="9" t="s">
         <v>12</v>
       </c>
@@ -1382,9 +1367,6 @@
       <c r="E8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="8">
-        <v>574.390537135822</v>
-      </c>
       <c r="H8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1411,9 +1393,6 @@
       <c r="E9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="8">
-        <v>554.65517930496901</v>
-      </c>
       <c r="H9" s="9" t="s">
         <v>12</v>
       </c>
@@ -1440,9 +1419,6 @@
       <c r="E10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="8">
-        <v>533.08495526082095</v>
-      </c>
       <c r="H10" s="9" t="s">
         <v>12</v>
       </c>
@@ -1469,9 +1445,6 @@
       <c r="E11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="8">
-        <v>551.38058849998595</v>
-      </c>
       <c r="H11" s="9" t="s">
         <v>12</v>
       </c>
@@ -1498,9 +1471,6 @@
       <c r="E12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="8">
-        <v>491.85541313285597</v>
-      </c>
       <c r="H12" s="9" t="s">
         <v>12</v>
       </c>
@@ -1527,9 +1497,6 @@
       <c r="E13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="8">
-        <v>532.70051044591696</v>
-      </c>
       <c r="H13" s="9" t="s">
         <v>12</v>
       </c>
@@ -1556,9 +1523,6 @@
       <c r="E14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="8">
-        <v>10000</v>
-      </c>
       <c r="H14" s="9" t="s">
         <v>12</v>
       </c>
@@ -1585,9 +1549,6 @@
       <c r="E15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="8">
-        <v>10000</v>
-      </c>
       <c r="H15" s="9" t="s">
         <v>12</v>
       </c>
@@ -1614,9 +1575,6 @@
       <c r="E16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="8">
-        <v>10000</v>
-      </c>
       <c r="H16" s="9" t="s">
         <v>12</v>
       </c>
@@ -1643,9 +1601,6 @@
       <c r="E17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="8">
-        <v>10000</v>
-      </c>
       <c r="H17" s="9" t="s">
         <v>12</v>
       </c>
@@ -1672,9 +1627,6 @@
       <c r="E18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="8">
-        <v>10000</v>
-      </c>
       <c r="H18" s="9" t="s">
         <v>12</v>
       </c>
@@ -1701,9 +1653,6 @@
       <c r="E19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="8">
-        <v>10000</v>
-      </c>
       <c r="H19" s="9" t="s">
         <v>12</v>
       </c>
@@ -1730,9 +1679,6 @@
       <c r="E20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="8">
-        <v>750.66677314294304</v>
-      </c>
       <c r="H20" s="9" t="s">
         <v>12</v>
       </c>
@@ -1759,9 +1705,6 @@
       <c r="E21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="8">
-        <v>760.52913468593795</v>
-      </c>
       <c r="H21" s="9" t="s">
         <v>12</v>
       </c>
@@ -1788,9 +1731,6 @@
       <c r="E22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="8">
-        <v>753.53060511443198</v>
-      </c>
       <c r="H22" s="9" t="s">
         <v>12</v>
       </c>
@@ -1817,9 +1757,6 @@
       <c r="E23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="8">
-        <v>823.972951445646</v>
-      </c>
       <c r="H23" s="9" t="s">
         <v>12</v>
       </c>
@@ -1846,9 +1783,6 @@
       <c r="E24" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="8">
-        <v>743.86346439805902</v>
-      </c>
       <c r="H24" s="9" t="s">
         <v>12</v>
       </c>
@@ -1875,9 +1809,6 @@
       <c r="E25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="8">
-        <v>771.21598480468799</v>
-      </c>
       <c r="H25" s="9" t="s">
         <v>12</v>
       </c>
@@ -1904,9 +1835,6 @@
       <c r="E26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="8">
-        <v>10000</v>
-      </c>
       <c r="H26" s="9" t="s">
         <v>12</v>
       </c>
@@ -1933,9 +1861,6 @@
       <c r="E27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="8">
-        <v>10000</v>
-      </c>
       <c r="H27" s="9" t="s">
         <v>12</v>
       </c>
@@ -1962,9 +1887,6 @@
       <c r="E28" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="8">
-        <v>10000</v>
-      </c>
       <c r="H28" s="9" t="s">
         <v>12</v>
       </c>
@@ -1992,9 +1914,6 @@
         <v>13</v>
       </c>
       <c r="F29" s="14"/>
-      <c r="G29" s="8">
-        <v>10000</v>
-      </c>
       <c r="H29" s="9" t="s">
         <v>12</v>
       </c>
@@ -2022,9 +1941,6 @@
         <v>13</v>
       </c>
       <c r="F30" s="14"/>
-      <c r="G30" s="8">
-        <v>10000</v>
-      </c>
       <c r="H30" s="9" t="s">
         <v>12</v>
       </c>
@@ -2082,7 +1998,7 @@
         <v>13</v>
       </c>
       <c r="G32" s="8">
-        <v>785.47104406828498</v>
+        <v>10000</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>12</v>
@@ -2111,7 +2027,7 @@
         <v>13</v>
       </c>
       <c r="G33" s="8">
-        <v>780.91141435054203</v>
+        <v>10000</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>12</v>
@@ -2140,7 +2056,7 @@
         <v>13</v>
       </c>
       <c r="G34" s="8">
-        <v>737.32977170251604</v>
+        <v>10000</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>12</v>
@@ -2169,7 +2085,7 @@
         <v>13</v>
       </c>
       <c r="G35" s="8">
-        <v>954.19754151374002</v>
+        <v>10000</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>12</v>
@@ -2198,7 +2114,7 @@
         <v>13</v>
       </c>
       <c r="G36" s="8">
-        <v>865.66566546456602</v>
+        <v>10000</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>12</v>
@@ -2227,7 +2143,7 @@
         <v>13</v>
       </c>
       <c r="G37" s="8">
-        <v>916.24805997644</v>
+        <v>10000</v>
       </c>
       <c r="H37" s="9" t="s">
         <v>12</v>
@@ -2346,7 +2262,7 @@
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="8">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>12</v>
@@ -2376,7 +2292,7 @@
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="8">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>12</v>
@@ -2406,7 +2322,7 @@
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="8">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>12</v>
@@ -2435,7 +2351,7 @@
         <v>13</v>
       </c>
       <c r="G44" s="8">
-        <v>642.46163906479205</v>
+        <v>10000</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>12</v>
@@ -2464,7 +2380,7 @@
         <v>13</v>
       </c>
       <c r="G45" s="8">
-        <v>654.03711406296998</v>
+        <v>10000</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>12</v>
@@ -2493,7 +2409,7 @@
         <v>13</v>
       </c>
       <c r="G46" s="8">
-        <v>645.44258691112395</v>
+        <v>10000</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>12</v>
@@ -2522,7 +2438,7 @@
         <v>13</v>
       </c>
       <c r="G47" s="8">
-        <v>891.17194251389799</v>
+        <v>10000</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>12</v>
@@ -2551,7 +2467,7 @@
         <v>13</v>
       </c>
       <c r="G48" s="8">
-        <v>835.20139961829796</v>
+        <v>10000</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>12</v>
@@ -2580,7 +2496,7 @@
         <v>13</v>
       </c>
       <c r="G49" s="8">
-        <v>876.88286096870002</v>
+        <v>10000</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>12</v>
@@ -2786,7 +2702,7 @@
         <v>13</v>
       </c>
       <c r="G56" s="8">
-        <v>154.10180409364099</v>
+        <v>10000</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>12</v>
@@ -2815,7 +2731,7 @@
         <v>13</v>
       </c>
       <c r="G57" s="8">
-        <v>154.009944921678</v>
+        <v>10000</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>12</v>
@@ -2844,7 +2760,7 @@
         <v>13</v>
       </c>
       <c r="G58" s="8">
-        <v>153.66645656718401</v>
+        <v>10000</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>12</v>
@@ -2873,7 +2789,7 @@
         <v>13</v>
       </c>
       <c r="G59" s="8">
-        <v>155.59488033231401</v>
+        <v>10000</v>
       </c>
       <c r="H59" s="9" t="s">
         <v>12</v>
@@ -2902,7 +2818,7 @@
         <v>13</v>
       </c>
       <c r="G60" s="8">
-        <v>154.89415224419099</v>
+        <v>10000</v>
       </c>
       <c r="H60" s="9" t="s">
         <v>12</v>
@@ -2931,7 +2847,7 @@
         <v>13</v>
       </c>
       <c r="G61" s="8">
-        <v>148.106906534091</v>
+        <v>10000</v>
       </c>
       <c r="H61" s="9" t="s">
         <v>12</v>
@@ -3050,7 +2966,7 @@
         <v>13</v>
       </c>
       <c r="G65" s="8">
-        <v>163.268971161054</v>
+        <v>10000</v>
       </c>
       <c r="H65" s="9" t="s">
         <v>12</v>
@@ -3079,7 +2995,7 @@
         <v>13</v>
       </c>
       <c r="G66" s="8">
-        <v>155.405277465583</v>
+        <v>10000</v>
       </c>
       <c r="H66" s="9" t="s">
         <v>12</v>
@@ -3108,7 +3024,7 @@
         <v>13</v>
       </c>
       <c r="G67" s="8">
-        <v>160.201937087711</v>
+        <v>10000</v>
       </c>
       <c r="H67" s="9" t="s">
         <v>12</v>
@@ -3137,7 +3053,7 @@
         <v>13</v>
       </c>
       <c r="G68" s="8">
-        <v>161.734488910111</v>
+        <v>10000</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>12</v>
@@ -3166,7 +3082,7 @@
         <v>13</v>
       </c>
       <c r="G69" s="8">
-        <v>158.74808630083501</v>
+        <v>10000</v>
       </c>
       <c r="H69" s="9" t="s">
         <v>12</v>
@@ -3195,7 +3111,7 @@
         <v>13</v>
       </c>
       <c r="G70" s="8">
-        <v>159.77408931656601</v>
+        <v>10000</v>
       </c>
       <c r="H70" s="9" t="s">
         <v>12</v>
@@ -3224,7 +3140,7 @@
         <v>13</v>
       </c>
       <c r="G71" s="8">
-        <v>163.21607432714899</v>
+        <v>10000</v>
       </c>
       <c r="H71" s="9" t="s">
         <v>12</v>
@@ -3253,7 +3169,7 @@
         <v>13</v>
       </c>
       <c r="G72" s="8">
-        <v>161.14014829524999</v>
+        <v>10000</v>
       </c>
       <c r="H72" s="9" t="s">
         <v>12</v>
@@ -3282,7 +3198,7 @@
         <v>13</v>
       </c>
       <c r="G73" s="8">
-        <v>160.148330487274</v>
+        <v>10000</v>
       </c>
       <c r="H73" s="9" t="s">
         <v>12</v>
@@ -3398,7 +3314,7 @@
         <v>13</v>
       </c>
       <c r="G77" s="8">
-        <v>150.18890950465499</v>
+        <v>10000</v>
       </c>
       <c r="H77" s="9" t="s">
         <v>12</v>
@@ -3427,7 +3343,7 @@
         <v>13</v>
       </c>
       <c r="G78" s="8">
-        <v>140.01651595281601</v>
+        <v>10000</v>
       </c>
       <c r="H78" s="9" t="s">
         <v>12</v>
@@ -3456,7 +3372,7 @@
         <v>13</v>
       </c>
       <c r="G79" s="8">
-        <v>141.41714859244399</v>
+        <v>10000</v>
       </c>
       <c r="H79" s="9" t="s">
         <v>12</v>
@@ -3485,7 +3401,7 @@
         <v>13</v>
       </c>
       <c r="G80" s="8">
-        <v>161.70099934784699</v>
+        <v>10000</v>
       </c>
       <c r="H80" s="9" t="s">
         <v>12</v>
@@ -3514,7 +3430,7 @@
         <v>13</v>
       </c>
       <c r="G81" s="8">
-        <v>147.43148904090799</v>
+        <v>10000</v>
       </c>
       <c r="H81" s="9" t="s">
         <v>12</v>
@@ -3543,7 +3459,7 @@
         <v>13</v>
       </c>
       <c r="G82" s="8">
-        <v>143.795529159468</v>
+        <v>10000</v>
       </c>
       <c r="H82" s="9" t="s">
         <v>12</v>
@@ -3572,7 +3488,7 @@
         <v>13</v>
       </c>
       <c r="G83" s="8">
-        <v>144.75302994894199</v>
+        <v>10000</v>
       </c>
       <c r="H83" s="9" t="s">
         <v>12</v>
@@ -3601,7 +3517,7 @@
         <v>13</v>
       </c>
       <c r="G84" s="8">
-        <v>134.59101726820001</v>
+        <v>10000</v>
       </c>
       <c r="H84" s="9" t="s">
         <v>12</v>
@@ -3630,7 +3546,7 @@
         <v>13</v>
       </c>
       <c r="G85" s="8">
-        <v>142.313807004057</v>
+        <v>10000</v>
       </c>
       <c r="H85" s="9" t="s">
         <v>12</v>
@@ -3746,7 +3662,7 @@
         <v>13</v>
       </c>
       <c r="G89" s="8">
-        <v>146.59479306730199</v>
+        <v>10000</v>
       </c>
       <c r="H89" s="9" t="s">
         <v>12</v>
@@ -3775,7 +3691,7 @@
         <v>13</v>
       </c>
       <c r="G90" s="8">
-        <v>147.28441698794501</v>
+        <v>10000</v>
       </c>
       <c r="H90" s="9" t="s">
         <v>12</v>
@@ -3807,7 +3723,7 @@
         <v>12</v>
       </c>
       <c r="G91" s="8">
-        <v>144.952941774717</v>
+        <v>10000</v>
       </c>
       <c r="H91" s="9" t="s">
         <v>12</v>
@@ -3839,7 +3755,7 @@
         <v>12</v>
       </c>
       <c r="G92" s="8">
-        <v>148.951321820771</v>
+        <v>10000</v>
       </c>
       <c r="H92" s="9" t="s">
         <v>12</v>
@@ -3871,7 +3787,7 @@
         <v>12</v>
       </c>
       <c r="G93" s="8">
-        <v>140.79854678555699</v>
+        <v>10000</v>
       </c>
       <c r="H93" s="9" t="s">
         <v>12</v>
@@ -3903,7 +3819,7 @@
         <v>12</v>
       </c>
       <c r="G94" s="8">
-        <v>110.420505022349</v>
+        <v>10000</v>
       </c>
       <c r="H94" s="9" t="s">
         <v>12</v>

</xml_diff>